<commit_message>
first check for ng-get in hmis module
</commit_message>
<xml_diff>
--- a/sql/employeesPenaltiesNames.xlsx
+++ b/sql/employeesPenaltiesNames.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>nameAr</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Adminstration Penality</t>
+  </si>
+  <si>
+    <t>عقوبة</t>
+  </si>
+  <si>
+    <t>عقوبه</t>
   </si>
 </sst>
 </file>
@@ -365,18 +371,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -384,7 +391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -392,12 +399,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug if employee dosn't  have allowenceslist or deductionsList
</commit_message>
<xml_diff>
--- a/sql/employeesPenaltiesNames.xlsx
+++ b/sql/employeesPenaltiesNames.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>nameAr</t>
   </si>
@@ -24,22 +24,316 @@
     <t>nameEn</t>
   </si>
   <si>
-    <t>جزاء اداري</t>
-  </si>
-  <si>
-    <t>جزاء  مالي</t>
-  </si>
-  <si>
-    <t>Financial Penality</t>
-  </si>
-  <si>
-    <t>Adminstration Penality</t>
-  </si>
-  <si>
-    <t>عقوبة</t>
-  </si>
-  <si>
-    <t>عقوبه</t>
+    <t>التأخر عن مواعيد الحضور للعمل أكثر من (30) دقيقة لغاية (60) دقيقة دون إذن أو عذر مقبول، إذا ترتب على ذلك تعطيل عمال آخرين</t>
+  </si>
+  <si>
+    <t>التأخر عن مواعيد الحضور للعمل أكثر من (15) دقيقة لغاية (30) دقيقة دون إذن أو عذر مقبول، إذا ترتب على ذلك تعطيل عمال آخرين</t>
+  </si>
+  <si>
+    <t>التأخر عن مواعيد الحضور للعمل لغاية (15) دقيقة دون إذن أو عذر مقبول، إذا لم يترتب على ذلك تعطيل عمال آخرين</t>
+  </si>
+  <si>
+    <t>اتأخر عن مواعيد الحضور للعمل لغاية (15) دقيقة دون إذن أو عذر مقبول، إذا ترتب على ذلك تعطيل عمال آخرين</t>
+  </si>
+  <si>
+    <t>التأخر عن مواعيد الحضور للعمل أكثر من  (15) دقيقة لغاية (30) دقيقة دون إذن أو عذر  مقبول، إذا لم يترتب على ذلك تعطيل عمال آخرين</t>
+  </si>
+  <si>
+    <t>التأخر عن مواعيد الحضور للعمل أكثر من  (30) دقيقة لغاية (60) دقيقة دون إذن أو عذر  مقبول، إذا لم يترتب على ذلك تعطيل عمال آخرين</t>
+  </si>
+  <si>
+    <t>التأخر عن مواعيد الحضور للعمل لمدة تزيد  على ساعة دون إذن أو عذر مقبول، سواء ترتب أو لم يترتب على ذلك تعطيل عمال آخرين</t>
+  </si>
+  <si>
+    <t>Late for work, 15 minutes or less without permission or a valid reason, if it did not cause delay to other employees</t>
+  </si>
+  <si>
+    <t>Late for work, 15 minutes or less without permission or a valid reason, if it caused delay to other employees</t>
+  </si>
+  <si>
+    <t>Late for work, 16-30 minutes without permission or a valid reason, if it did not cause delay to other employees</t>
+  </si>
+  <si>
+    <t>Late for work, 16-30 minutes without permission or a valid reason, if it caused delay to other employees</t>
+  </si>
+  <si>
+    <t>Late for work, 31-60 minutes without permission or a valid reason, if it did not cause delay to other employees</t>
+  </si>
+  <si>
+    <t>Late for work, 31-60 minutes without permission or a valid reason, if it caused delay other employees</t>
+  </si>
+  <si>
+    <t>Late for work more than 60 minutes without permission or a valid reason, regardless of whether or not tardiness caused delay to other employees</t>
+  </si>
+  <si>
+    <t>ترك العمل، أو الانصراف قبل الميعاد دون إذن  أو عذر مقبول بما لا يتجاوز (15) دقيقة</t>
+  </si>
+  <si>
+    <t>ترك العمل، أو الانصراف قبل الميعاد دون إذن أو عذر مقبول بما يتجاوز (15) دقيقة</t>
+  </si>
+  <si>
+    <t>البقاء في أماكن العمل أو العودة اليها بعد انتهاء مواعيد العمل دون إذن مسبق</t>
+  </si>
+  <si>
+    <t>مغادرة مقر العمل دون التوقيع على كشف  الحضور والانصراف (ان وجد)</t>
+  </si>
+  <si>
+    <t>الغياب دون اذن كتابي أو عذر مقبول لمدة يوم  (1) واحد خلال السنة العقدية الواحدة</t>
+  </si>
+  <si>
+    <t>الغياب المتصل دون اذن كتابي أو عذر مقبول من يومين إلى ستة (2 - 6 ) أيام خلال السنة العقدية الواحدة</t>
+  </si>
+  <si>
+    <t>Absence without written permission or justified excuse for (2 to 6) days within a contract year</t>
+  </si>
+  <si>
+    <t>Absence without written permission or justified excuse for one (1) day within a contract year</t>
+  </si>
+  <si>
+    <t>Departing from the jobsite without passing through a timekeeping check (if applicable)</t>
+  </si>
+  <si>
+    <t>Remaining at the jobsite or returning to it after end of workday without a permission</t>
+  </si>
+  <si>
+    <t>Departing from work more than 15 minutes early without permission or a valid reason</t>
+  </si>
+  <si>
+    <t>Departing from work 1-15 minutes early without permission or a valid reason</t>
+  </si>
+  <si>
+    <t>الغياب المتصل دون اذن كتابي أو عذر مقبول من سبعة أيام إلى عشرة (7 - 10) أيام خلال السنة العقدية الواحدة</t>
+  </si>
+  <si>
+    <t>الانقطاع عن العمل دون سبب مشروع مدة تزيد ً متصلة خلال السنة عن (15) خمسة عشر يوما العقدية الواحدة</t>
+  </si>
+  <si>
+    <t>الغياب المتصل دون اذن كتابي أو عذر مقبول  إلى أربعة عشر يوما من أحد عشر يوما (11 – 14 )خلال السنة العقدية الواحدة</t>
+  </si>
+  <si>
+    <t>الغياب المتق تزيد في طع دون سبب مشروع مددا ً خلال السنة مجموعها على ثلاثين (30) يوما العقدية الواحدة</t>
+  </si>
+  <si>
+    <t>Absence without written permission or justified excuse for (7 to 10) days within a contract year</t>
+  </si>
+  <si>
+    <t>Absence without written permission or justified excuse for (11 to 14) days within a contract year</t>
+  </si>
+  <si>
+    <t>Absence without written permission or justified excuse for more than fifteen (15) consecutive days within a contract year</t>
+  </si>
+  <si>
+    <t>Intermittent absence without proper  authority for periods totalling more than thirty (30) days within a contract year</t>
+  </si>
+  <si>
+    <t>Being in a place other than the jobsite without proper justification</t>
+  </si>
+  <si>
+    <t>Receiving visitors not related to work in the jobsite without management permission</t>
+  </si>
+  <si>
+    <t>Use of Program tools, equipment or  supply materials for private purposes without permission</t>
+  </si>
+  <si>
+    <t>Interfering with the work, which is not within his/her purview or had not been assigned to him/her</t>
+  </si>
+  <si>
+    <t>Exit and entry of non-allocated areas</t>
+  </si>
+  <si>
+    <t>Negligence of cleaning and maintenance of machinery and equipment or failure to report Program damage when it occurs</t>
+  </si>
+  <si>
+    <t>Failure to keep maintenance tools in allotted places after completion of the work</t>
+  </si>
+  <si>
+    <t>Disrupting or destroying ads or announcements related to work</t>
+  </si>
+  <si>
+    <t>Negligence of assigned custody (cars,machines … etc)</t>
+  </si>
+  <si>
+    <t>التواجد دون مبرر في غير مكان العمل  المخصص للعامل اثناء وقت الدوام</t>
+  </si>
+  <si>
+    <t>استقبال زائرين في غير أمور عمل المنشأة في أماكن العمل دون اذن من الإدارة</t>
+  </si>
+  <si>
+    <t>ستعمال آلات ومعدات وأدوات المنشأة لأغراض خاصة دون إذن</t>
+  </si>
+  <si>
+    <t>تدخل العامل دون وجه حق في أي عمل ليس في اختصاصه أو لم يعهد به اليه</t>
+  </si>
+  <si>
+    <t>الخروج أو الدخول من غير المكان المخصص لذلك</t>
+  </si>
+  <si>
+    <t>الإهمال في تنظيف الآلات وصيانتها أو عدم  العناية بها أو عدم التبليغ عن ما بها من خلل</t>
+  </si>
+  <si>
+    <t>عدم وضع أدوات الإصلاح والصيانة واللوازم الاخرى في الأماكن المخصصة لها بعد الانتهاء من العمل</t>
+  </si>
+  <si>
+    <t>تمزيق أو اتلاف إعلانات أو بلاغات إدارة  المنشأة</t>
+  </si>
+  <si>
+    <t>الأكل في مكان العمل أو غير المكان المعد له أو في غير أوقات الراحة</t>
+  </si>
+  <si>
+    <t>النوم أثناء العمل</t>
+  </si>
+  <si>
+    <t>النوم في الحالات التي تستدعي يقظة مستمرة</t>
+  </si>
+  <si>
+    <t>التلاعب في إثبات الحضور والانصراف</t>
+  </si>
+  <si>
+    <t>عدم إطاعة الأوامر العادية الخاصة بالعمل أو عدم تنفيذ التعليمات الخاصة بالعمل والمعلقة في مكان ظاهر</t>
+  </si>
+  <si>
+    <t>التسكع/ التجول أو وجود العامل في غير مكان  عمله أثناء ساعات العمل</t>
+  </si>
+  <si>
+    <t>الإهمال في العهد التي بحوزته، مثال (سيارات، آلات، أجهزة، معدات، أدوات، الخ)</t>
+  </si>
+  <si>
+    <t>التحريض على مخالفة الأوامر والتعليمات الخطية الخاصة بالعمل</t>
+  </si>
+  <si>
+    <t>التدخين في الأماكن المحظورة والمعلن عنها  للمحافظة على سلامة العمال والمنشأة</t>
+  </si>
+  <si>
+    <t>الإهمال أو التهاون في العمل الذي قد ينشأ عنه ضرر في صحة العمال أو سلامتهم او في المواد أو الأدوات والأجهزة</t>
+  </si>
+  <si>
+    <t>الإهمال أو الفشل في الإبلاغ عن وقوع أضرار  لممتلكات البرنامج فور حدوثها</t>
+  </si>
+  <si>
+    <t>عدم الالتزام بارتداء بطاقة الهوية في موقع العمل</t>
+  </si>
+  <si>
+    <t>Eating in an unauthorized place or at an unauthorized time</t>
+  </si>
+  <si>
+    <t>Sleeping during working hours</t>
+  </si>
+  <si>
+    <t>Sleeping on duties that required high alertness</t>
+  </si>
+  <si>
+    <t>Wandering about to places other than to place assigned to work during working hours</t>
+  </si>
+  <si>
+    <t>Manipulation in attendance and time records</t>
+  </si>
+  <si>
+    <t>Disobedience of normal work orders, or not following work instructions when these instructions are posted in a conspicuous place at the jobsite</t>
+  </si>
+  <si>
+    <t>To incite others to disobey orders and written instructions relating to work</t>
+  </si>
+  <si>
+    <t>Smoking in restricted areas</t>
+  </si>
+  <si>
+    <t>Negligence or failure to perform a task which could endanger the safety of others, Program material or equipment</t>
+  </si>
+  <si>
+    <t>Negligence or failure to report Program damage when it occurs</t>
+  </si>
+  <si>
+    <t>Non-compliance with ID / Badge wearing while on the Program site</t>
+  </si>
+  <si>
+    <t>التشاجر مع الزملاء أو مع الغير، أو إحداث  مشاغبات في مكان العمل</t>
+  </si>
+  <si>
+    <t>التمارض أو ادعاء العامل كذبا أنه أصيب أثناء العمل أو بسببه</t>
+  </si>
+  <si>
+    <t>الامتناع عن إجراء الكشف الطبي عند طلب طبيب المنشأة، أو رفض اتباع التعليمات الطبية أثناء العلاج</t>
+  </si>
+  <si>
+    <t>مخالفة التعليمات الصحية المعلقة بأماكن العمل</t>
+  </si>
+  <si>
+    <t>الكتابة على جدران المنشأة أو لصق إعلانات عليها</t>
+  </si>
+  <si>
+    <t>رفض التفتيش الإداري عند الانصراف</t>
+  </si>
+  <si>
+    <t>عدم تسليم النقود المحصلة لحساب المنشأة في  المواعيد المحددة دون تبرير مقبول</t>
+  </si>
+  <si>
+    <t>الامتناع عن ارتداء الملابس والأجهزة المقررة  للوقاية وللسلامة</t>
+  </si>
+  <si>
+    <t>Fighting or causing trouble on the worksite</t>
+  </si>
+  <si>
+    <t>Malingering or falsely claims of work-related injuries or injuries occurred during working hours</t>
+  </si>
+  <si>
+    <t>Refusing to submit to a physical examination by the Program Physician, or following the medical instructions during treatment</t>
+  </si>
+  <si>
+    <t>Failure to follow health regulations/ instructions posted in a conspicuous place at the job site</t>
+  </si>
+  <si>
+    <t>Writing on walls or posting unauthorized papers or posters</t>
+  </si>
+  <si>
+    <t>Refusing to submit to inspection when departing the job site</t>
+  </si>
+  <si>
+    <t>Failure to hand over the collected money for the organization at the deadline without an acceptable justification</t>
+  </si>
+  <si>
+    <t>Refrain from wearing necessary clothing and equipment for prevention and safety</t>
+  </si>
+  <si>
+    <t>عمد الخلوة مع الجنس الآخر في أماكن العمل</t>
+  </si>
+  <si>
+    <t>الإيحاء للآخرين بما يخدش الحياء قولا أو فعلا</t>
+  </si>
+  <si>
+    <t>الاعتداء على زملاء العمل بالقول أو الإشارة أو باستعمال وسائل الاتصال الالكترونية بالشتم أو التحقير</t>
+  </si>
+  <si>
+    <t>الاعتداء بالإيذاء الجسدي على زملاء العمل أو على غيرهم بطريقة إباحية</t>
+  </si>
+  <si>
+    <t>الاعتداء الجسدي أو القولي أو بأي وسيلة من وسائل الاتصال الالكترونية على صاحب العمل أو المدير المسئول أو أحد الرؤساء أثناء العمل أو بسببه</t>
+  </si>
+  <si>
+    <t>تقديم بلاغ أو شكوى كيدية</t>
+  </si>
+  <si>
+    <t>عدم الامتثال لطلب لجنة التحقيق بالحضور</t>
+  </si>
+  <si>
+    <t>Intentional seclusion (khalwa) with the opposite gender in the workplace</t>
+  </si>
+  <si>
+    <t>Inappropriate language and gestures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assaulting colleagues by using language, gesture, or through electronic communication channel to convey profanity or insult</t>
+  </si>
+  <si>
+    <t>Harassment whether sexual or physical to co-workers or others</t>
+  </si>
+  <si>
+    <t>Assaulting physically, verbally or through electronic communication channels to any of the managers or stakeholders/employer</t>
+  </si>
+  <si>
+    <t>False or malicious complaint or incident report</t>
+  </si>
+  <si>
+    <t>Failure to respond, attend, testify or give statement as summoned by Investigation/Committee</t>
   </si>
 </sst>
 </file>
@@ -75,8 +369,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,19 +668,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="104" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,30 +689,420 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" t="s">
-        <v>7</v>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>